<commit_message>
I think it's done
</commit_message>
<xml_diff>
--- a/contacts_formatted.xlsx
+++ b/contacts_formatted.xlsx
@@ -247,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
@@ -334,10 +334,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="2" fillId="3" fontId="1" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="4" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -947,29 +943,37 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="n"/>
-      <c r="B7" s="36" t="inlineStr">
+      <c r="B7" s="33" t="inlineStr">
         <is>
           <t>89797239729</t>
         </is>
       </c>
-      <c r="C7" s="37" t="n"/>
+      <c r="C7" s="35" t="n"/>
       <c r="D7" s="34" t="n"/>
       <c r="E7" s="34" t="n"/>
       <c r="F7" s="35" t="n"/>
-      <c r="G7" s="35" t="n"/>
+      <c r="G7" s="35" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="32" t="n"/>
-      <c r="B8" s="36" t="inlineStr">
+      <c r="B8" s="33" t="inlineStr">
         <is>
           <t>98982380</t>
         </is>
       </c>
-      <c r="C8" s="37" t="n"/>
+      <c r="C8" s="35" t="n"/>
       <c r="D8" s="34" t="n"/>
       <c r="E8" s="34" t="n"/>
       <c r="F8" s="35" t="n"/>
-      <c r="G8" s="35" t="n"/>
+      <c r="G8" s="35" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="32" t="inlineStr">
@@ -989,7 +993,7 @@
         </is>
       </c>
       <c r="E9" s="34" t="n"/>
-      <c r="F9" s="38" t="n"/>
+      <c r="F9" s="36" t="n"/>
       <c r="G9" s="35" t="inlineStr">
         <is>
           <t>other</t>
@@ -1027,7 +1031,7 @@
         </is>
       </c>
       <c r="E11" s="34" t="n"/>
-      <c r="F11" s="38" t="n"/>
+      <c r="F11" s="36" t="n"/>
       <c r="G11" s="35" t="n"/>
     </row>
     <row r="12">
@@ -1081,29 +1085,32 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="32" t="n"/>
-      <c r="B14" s="36" t="inlineStr">
+      <c r="A14" s="18" t="n"/>
+      <c r="B14" s="24" t="inlineStr">
         <is>
           <t>988-708-9782</t>
         </is>
       </c>
-      <c r="C14" s="37" t="n"/>
-      <c r="D14" s="34" t="inlineStr">
+      <c r="D14" s="6" t="inlineStr">
         <is>
           <t>another</t>
         </is>
       </c>
-      <c r="E14" s="34" t="inlineStr">
+      <c r="E14" s="6" t="inlineStr">
         <is>
           <t>person</t>
         </is>
       </c>
-      <c r="F14" s="35" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>9887089782</t>
         </is>
       </c>
-      <c r="G14" s="35" t="n"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="18" t="n"/>

</xml_diff>